<commit_message>
add proj to proto
</commit_message>
<xml_diff>
--- a/qlib/qtx/allTest/alltest.xlsx
+++ b/qlib/qtx/allTest/alltest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\edev\private_projects\btick2\src\qlib\qtx\allTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10000001_{ACA65D83-4392-4E3B-BD70-40DBED09BDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46229093-5576-4F3B-A0F6-D6CB68800EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19210" yWindow="9940" windowWidth="19140" windowHeight="20650" xr2:uid="{05851AF6-74E8-4555-9905-605044867CE4}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -184,36 +183,36 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv_bc3933114a0a4596983e4461806c12b9">
+    <main first="rtdsrv_720d4a865ea548f4bafec331ab153979">
       <tp>
-        <v>2356</v>
+        <v>625</v>
         <stp/>
-        <stp>9_kpi_heartbeat.2</stp>
+        <stp>9_kpi_heartbeat.3</stp>
         <tr r="N2" s="1"/>
       </tp>
     </main>
-    <main first="rtdsrv_1d0352ecb61c46df8926e667f70994d6">
+    <main first="rtdsrv_720d4a865ea548f4bafec331ab153979">
       <tp t="s">
-        <v>08:11:51</v>
+        <v>18:35:28 (ConnectData)</v>
+        <stp/>
+        <stp>9_kpi_rsummary.3</stp>
+        <tr r="M5" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv_7cdf0c5fb9834086b8face2482385385">
+      <tp t="s">
+        <v>18:47:02</v>
         <stp/>
         <stp>rtdclock.rtdclockserver</stp>
         <tr r="C11" s="2"/>
       </tp>
     </main>
-    <main first="rtdsrv_bc3933114a0a4596983e4461806c12b9">
+    <main first="rtdsrv_720d4a865ea548f4bafec331ab153979">
       <tp>
-        <v>2357</v>
+        <v>625</v>
         <stp/>
-        <stp>9_kpi_status.2</stp>
+        <stp>9_kpi_status.3</stp>
         <tr r="N3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv_bc3933114a0a4596983e4461806c12b9">
-      <tp>
-        <v>2174</v>
-        <stp/>
-        <stp>9_kpi_rsummary.2</stp>
-        <tr r="M5" s="1"/>
       </tp>
     </main>
   </volType>
@@ -537,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7ECE94-EB29-433D-B0C9-40CC7ADB27D3}">
-  <dimension ref="B2:S9"/>
+  <dimension ref="B2:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,7 +555,7 @@
     <col min="18" max="19" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -585,7 +584,7 @@
         <v>6</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M2" t="s">
         <v>13</v>
@@ -598,10 +597,10 @@
         <v>*</v>
       </c>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B3" t="str">
         <f>"9_kpi_heartbeat."&amp;K3</f>
-        <v>9_kpi_heartbeat.2</v>
+        <v>9_kpi_heartbeat.3</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -620,11 +619,11 @@
       </c>
       <c r="J3" t="str" cm="1">
         <f t="array" ref="J3">_xll.qxl_open_subscriber(B3,C3,D3,E3,F3,G3,H3,I3)</f>
-        <v>9_kpi_heartbeat.2</v>
+        <v>9_kpi_heartbeat.3</v>
       </c>
       <c r="K3">
         <f>$K$2</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M3" t="s">
         <v>14</v>
@@ -637,10 +636,10 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B4" t="str">
         <f>"9_kpi_status."&amp;K4</f>
-        <v>9_kpi_status.2</v>
+        <v>9_kpi_status.3</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -659,17 +658,17 @@
       </c>
       <c r="J4" t="str" cm="1">
         <f t="array" ref="J4">_xll.qxl_open_subscriber(B4,C4,D4,E4,F4,G4,H4,I4)</f>
-        <v>9_kpi_status.2</v>
+        <v>9_kpi_status.3</v>
       </c>
       <c r="K4">
         <f>$K$2</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" t="str">
         <f>"9_kpi_rsummary."&amp;K5</f>
-        <v>9_kpi_rsummary.2</v>
+        <v>9_kpi_rsummary.3</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -688,125 +687,15 @@
       </c>
       <c r="J5" t="str" cm="1">
         <f t="array" ref="J5">_xll.qxl_open_subscriber(B5,C5,D5,E5,F5,G5,H5,I5)</f>
-        <v>9_kpi_rsummary.2</v>
+        <v>9_kpi_rsummary.3</v>
       </c>
       <c r="K5">
         <f>$K$2</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M5" t="str" cm="1">
-        <f t="array" ref="M5:S9">_xll.qxl_subscribe(J5)</f>
-        <v>sha</v>
-      </c>
-      <c r="N5" t="str">
-        <v>uid</v>
-      </c>
-      <c r="O5" t="str">
-        <v>cnt</v>
-      </c>
-      <c r="P5" t="str">
-        <v>pass</v>
-      </c>
-      <c r="Q5" t="str">
-        <v>pass_ratio</v>
-      </c>
-      <c r="R5" t="str">
-        <v>stime</v>
-      </c>
-      <c r="S5" t="str">
-        <v>dtime</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="M6" t="str">
-        <v>3e66558cff</v>
-      </c>
-      <c r="N6" t="str">
-        <v>dbmaint1.testCase_after</v>
-      </c>
-      <c r="O6">
-        <v>4</v>
-      </c>
-      <c r="P6">
-        <v>4</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>45771.339371377311</v>
-      </c>
-      <c r="S6">
-        <v>5.777083333333333E-8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="M7" t="str">
-        <v>3e66558cff</v>
-      </c>
-      <c r="N7" t="str">
-        <v>dbmaint1.testCase_before</v>
-      </c>
-      <c r="O7">
-        <v>4</v>
-      </c>
-      <c r="P7">
-        <v>4</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>45771.339371249996</v>
-      </c>
-      <c r="S7">
-        <v>1.0532407407407408E-9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="M8" t="str">
-        <v>3e66558cff</v>
-      </c>
-      <c r="N8" t="str">
-        <v>dbmaint1</v>
-      </c>
-      <c r="O8">
-        <v>25</v>
-      </c>
-      <c r="P8">
-        <v>25</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8">
-        <v>45771.339371249996</v>
-      </c>
-      <c r="S8">
-        <v>4.4064814814814815E-7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="M9" t="str">
-        <v>3e66558cff</v>
-      </c>
-      <c r="N9" t="str">
-        <v>dbmaint1.before</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>45771.339371226852</v>
-      </c>
-      <c r="S9">
-        <v>1.9953703703703702E-8</v>
+        <f t="array" ref="M5">_xll.qxl_subscribe(J5)</f>
+        <v>18:35:28 (ConnectData)</v>
       </c>
     </row>
   </sheetData>
@@ -939,7 +828,7 @@
       </c>
       <c r="C11" t="str" cm="1">
         <f t="array" ref="C11">_xll.qxl_clock()</f>
-        <v>08:11:51</v>
+        <v>18:47:02</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>

</xml_diff>

<commit_message>
add readme and license file
</commit_message>
<xml_diff>
--- a/qlib/qtx/allTest/alltest.xlsx
+++ b/qlib/qtx/allTest/alltest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\edev\private_projects\btick2\src\qlib\qtx\allTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF9BA8C-91D8-49E8-BC6A-DC351930D227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA065B6-CEEF-41AB-B6ED-0CA4394F3FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19210" yWindow="9940" windowWidth="19140" windowHeight="20650" xr2:uid="{05851AF6-74E8-4555-9905-605044867CE4}"/>
   </bookViews>
@@ -185,7 +185,7 @@
   <volType type="realTimeData">
     <main first="rtdsrv_8797f8e4b15e48b5a88d17e9ea5eaf84">
       <tp>
-        <v>22</v>
+        <v>14008</v>
         <stp/>
         <stp>9_kpi_heartbeat.3</stp>
         <tr r="N2" s="1"/>
@@ -193,7 +193,7 @@
     </main>
     <main first="rtdsrv_8915e47b95ff4eeb89985ec191dd01ba">
       <tp t="s">
-        <v>07:45:00</v>
+        <v>12:00:24</v>
         <stp/>
         <stp>rtdclock.rtdclockserver</stp>
         <tr r="C11" s="2"/>
@@ -201,13 +201,13 @@
     </main>
     <main first="rtdsrv_8797f8e4b15e48b5a88d17e9ea5eaf84">
       <tp>
-        <v>8</v>
+        <v>1059</v>
         <stp/>
         <stp>9_kpi_rsummary.3</stp>
         <tr r="M5" s="1"/>
       </tp>
       <tp>
-        <v>22</v>
+        <v>14009</v>
         <stp/>
         <stp>9_kpi_status.3</stp>
         <tr r="N3" s="1"/>
@@ -537,7 +537,7 @@
   <dimension ref="B2:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,10 +589,10 @@
       </c>
       <c r="N2" t="str" cm="1">
         <f t="array" ref="N2:O2">_xll.qxl_subscribe(J3)</f>
+        <v>*</v>
+      </c>
+      <c r="O2" t="str">
         <v/>
-      </c>
-      <c r="O2" t="str">
-        <v>*</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.35">
@@ -716,7 +716,7 @@
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="M6" t="str">
-        <v>7f91cdad31</v>
+        <v>0eff36d46c</v>
       </c>
       <c r="N6" t="str">
         <v>adf1.testCase_after</v>
@@ -731,15 +731,15 @@
         <v>1</v>
       </c>
       <c r="R6">
-        <v>45799.322774375003</v>
+        <v>45799.338085995369</v>
       </c>
       <c r="S6">
-        <v>5.0925925925925924E-11</v>
+        <v>5.2083333333333334E-11</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="M7" t="str">
-        <v>7f91cdad31</v>
+        <v>0eff36d46c</v>
       </c>
       <c r="N7" t="str">
         <v>adf1.testCase_before</v>
@@ -754,15 +754,15 @@
         <v>1</v>
       </c>
       <c r="R7">
-        <v>45799.322774293978</v>
+        <v>45799.338085902775</v>
       </c>
       <c r="S7">
-        <v>2.8703703703703705E-10</v>
+        <v>2.6620370370370369E-10</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="M8" t="str">
-        <v>7f91cdad31</v>
+        <v>0eff36d46c</v>
       </c>
       <c r="N8" t="str">
         <v>adf1</v>
@@ -777,15 +777,15 @@
         <v>1</v>
       </c>
       <c r="R8">
-        <v>45799.322774293978</v>
+        <v>45799.338085902775</v>
       </c>
       <c r="S8">
-        <v>7.4229166666666667E-8</v>
+        <v>8.0401620370370376E-8</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.35">
       <c r="M9" t="str">
-        <v>7f91cdad31</v>
+        <v>0eff36d46c</v>
       </c>
       <c r="N9" t="str">
         <v>adf1.before</v>
@@ -800,15 +800,15 @@
         <v>1</v>
       </c>
       <c r="R9">
-        <v>45799.322774282409</v>
+        <v>45799.338085891206</v>
       </c>
       <c r="S9">
-        <v>1.4030092592592593E-8</v>
+        <v>1.3822916666666667E-8</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="M10" t="str">
-        <v>7f91cdad31</v>
+        <v>0eff36d46c</v>
       </c>
       <c r="N10" t="str">
         <v>proto1.testCase_after</v>
@@ -823,15 +823,15 @@
         <v>1</v>
       </c>
       <c r="R10">
-        <v>45799.322774282409</v>
+        <v>45799.338085891206</v>
       </c>
       <c r="S10">
-        <v>7.9861111111111111E-11</v>
+        <v>7.291666666666666E-11</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="M11" t="str">
-        <v>7f91cdad31</v>
+        <v>0eff36d46c</v>
       </c>
       <c r="N11" t="str">
         <v>proto1.testCase_before</v>
@@ -846,15 +846,15 @@
         <v>1</v>
       </c>
       <c r="R11">
-        <v>45799.322774247688</v>
+        <v>45799.338085868054</v>
       </c>
       <c r="S11">
-        <v>1.4004629629629631E-10</v>
+        <v>1.4583333333333332E-10</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.35">
       <c r="M12" t="str">
-        <v>7f91cdad31</v>
+        <v>0eff36d46c</v>
       </c>
       <c r="N12" t="str">
         <v>proto1</v>
@@ -869,15 +869,15 @@
         <v>1</v>
       </c>
       <c r="R12">
-        <v>45799.322774247688</v>
+        <v>45799.338085868054</v>
       </c>
       <c r="S12">
-        <v>1.8699074074074075E-8</v>
+        <v>1.6907407407407407E-8</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="M13" t="str">
-        <v>7f91cdad31</v>
+        <v>0eff36d46c</v>
       </c>
       <c r="N13" t="str">
         <v>proto1.before</v>
@@ -892,10 +892,10 @@
         <v>1</v>
       </c>
       <c r="R13">
-        <v>45799.322774236112</v>
+        <v>45799.338085844909</v>
       </c>
       <c r="S13">
-        <v>1.5086805555555555E-8</v>
+        <v>1.6817129629629629E-8</v>
       </c>
     </row>
   </sheetData>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="C11" t="str" cm="1">
         <f t="array" ref="C11">_xll.qxl_clock()</f>
-        <v>07:45:00</v>
+        <v>12:00:24</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>

</xml_diff>